<commit_message>
Before the folder rearrangement
We are trying to organize the figures for the publication.
</commit_message>
<xml_diff>
--- a/4_example/case_study_1.0/4_additional_plots/nc100.xlsx
+++ b/4_example/case_study_1.0/4_additional_plots/nc100.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkim333\Documents\GitHub\toPSAil\4_example\case_study_1.0\4_additional_plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A9046C-813D-4F9E-B063-2BC5F849DAE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4071D8F-A743-463E-8110-A120645B6B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{0ED74958-54E0-524A-BD2C-DFF2C3A96A3A}"/>
   </bookViews>
@@ -435,10 +435,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>2.5388425480973199E-5</v>
+        <v>2.5388317927472199E-5</v>
       </c>
       <c r="C2" s="1">
-        <v>9.1393660448066703E-5</v>
+        <v>9.1393273275252102E-5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -446,10 +446,10 @@
         <v>0.76969696969696999</v>
       </c>
       <c r="B3" s="1">
-        <v>2.5388425480973199E-5</v>
+        <v>2.5388317927472199E-5</v>
       </c>
       <c r="C3" s="1">
-        <v>9.1393660448066703E-5</v>
+        <v>9.1393273275252102E-5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -457,10 +457,10 @@
         <v>1.53939393939394</v>
       </c>
       <c r="B4" s="1">
-        <v>2.5388425480973199E-5</v>
+        <v>2.5388317927472199E-5</v>
       </c>
       <c r="C4" s="1">
-        <v>9.1393660448066703E-5</v>
+        <v>9.1393273275252102E-5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -468,10 +468,10 @@
         <v>2.30909090909091</v>
       </c>
       <c r="B5" s="1">
-        <v>2.5388425480973199E-5</v>
+        <v>2.5388317927472199E-5</v>
       </c>
       <c r="C5" s="1">
-        <v>9.1393660448066703E-5</v>
+        <v>9.1393273275252102E-5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -479,10 +479,10 @@
         <v>3.07878787878788</v>
       </c>
       <c r="B6" s="1">
-        <v>2.5388425480973199E-5</v>
+        <v>2.5388317927472199E-5</v>
       </c>
       <c r="C6" s="1">
-        <v>9.1393660448066595E-5</v>
+        <v>9.1393273275252102E-5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -490,10 +490,10 @@
         <v>3.84848484848485</v>
       </c>
       <c r="B7" s="1">
-        <v>2.5388425480973199E-5</v>
+        <v>2.5388317927472199E-5</v>
       </c>
       <c r="C7" s="1">
-        <v>9.1393660448066595E-5</v>
+        <v>9.1393273275252102E-5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -501,10 +501,10 @@
         <v>4.6181818181818199</v>
       </c>
       <c r="B8" s="1">
-        <v>2.5388425480973199E-5</v>
+        <v>2.5388317927472199E-5</v>
       </c>
       <c r="C8" s="1">
-        <v>9.1393660448066595E-5</v>
+        <v>9.1393273275252102E-5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -512,10 +512,10 @@
         <v>5.3878787878787904</v>
       </c>
       <c r="B9" s="1">
-        <v>2.5388425480973199E-5</v>
+        <v>2.5388317927472199E-5</v>
       </c>
       <c r="C9" s="1">
-        <v>9.1393660448066595E-5</v>
+        <v>9.1393273275252102E-5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -523,10 +523,10 @@
         <v>6.1575757575757599</v>
       </c>
       <c r="B10" s="1">
-        <v>2.5388425480973301E-5</v>
+        <v>2.5388317927472199E-5</v>
       </c>
       <c r="C10" s="1">
-        <v>9.1393660448066595E-5</v>
+        <v>9.1393273275252102E-5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -534,10 +534,10 @@
         <v>6.9272727272727304</v>
       </c>
       <c r="B11" s="1">
-        <v>2.5388425480973301E-5</v>
+        <v>2.5388317927472199E-5</v>
       </c>
       <c r="C11" s="1">
-        <v>9.13936604480665E-5</v>
+        <v>9.1393273275252102E-5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -545,10 +545,10 @@
         <v>7.6969696969696999</v>
       </c>
       <c r="B12" s="1">
-        <v>2.5388425480973301E-5</v>
+        <v>2.53883179274723E-5</v>
       </c>
       <c r="C12" s="1">
-        <v>9.13936604480665E-5</v>
+        <v>9.1393273275252102E-5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -556,10 +556,10 @@
         <v>8.4666666666666703</v>
       </c>
       <c r="B13" s="1">
-        <v>2.5388425480973301E-5</v>
+        <v>2.5388317927472199E-5</v>
       </c>
       <c r="C13" s="1">
-        <v>9.13936604480665E-5</v>
+        <v>9.1393273275251993E-5</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -567,10 +567,10 @@
         <v>9.2363636363636399</v>
       </c>
       <c r="B14" s="1">
-        <v>2.5388425480973301E-5</v>
+        <v>2.53883179274723E-5</v>
       </c>
       <c r="C14" s="1">
-        <v>9.13936604480665E-5</v>
+        <v>9.1393273275251993E-5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -578,10 +578,10 @@
         <v>10.006060606060601</v>
       </c>
       <c r="B15" s="1">
-        <v>2.5388425480973301E-5</v>
+        <v>2.53883179274723E-5</v>
       </c>
       <c r="C15" s="1">
-        <v>9.13936604480665E-5</v>
+        <v>9.1393273275251993E-5</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -589,10 +589,10 @@
         <v>10.7757575757576</v>
       </c>
       <c r="B16" s="1">
-        <v>2.5388425480973301E-5</v>
+        <v>2.53883179274723E-5</v>
       </c>
       <c r="C16" s="1">
-        <v>9.13936604480665E-5</v>
+        <v>9.1393273275251993E-5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -600,10 +600,10 @@
         <v>11.545454545454501</v>
       </c>
       <c r="B17" s="1">
-        <v>2.5388425480973301E-5</v>
+        <v>2.53883179274723E-5</v>
       </c>
       <c r="C17" s="1">
-        <v>9.13936604480665E-5</v>
+        <v>9.1393273275251993E-5</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -611,10 +611,10 @@
         <v>12.3151515151515</v>
       </c>
       <c r="B18" s="1">
-        <v>2.5388425480973301E-5</v>
+        <v>2.53883179274723E-5</v>
       </c>
       <c r="C18" s="1">
-        <v>9.13936604480665E-5</v>
+        <v>9.1393273275251993E-5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -622,10 +622,10 @@
         <v>13.0848484848485</v>
       </c>
       <c r="B19" s="1">
-        <v>2.5388425480973301E-5</v>
+        <v>2.53883179274723E-5</v>
       </c>
       <c r="C19" s="1">
-        <v>9.1393660448066405E-5</v>
+        <v>9.1393273275251993E-5</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -633,10 +633,10 @@
         <v>13.8545454545455</v>
       </c>
       <c r="B20" s="1">
-        <v>2.5388425480973301E-5</v>
+        <v>2.53883179274723E-5</v>
       </c>
       <c r="C20" s="1">
-        <v>9.1393660448066405E-5</v>
+        <v>9.1393273275251993E-5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -644,10 +644,10 @@
         <v>14.6242424242424</v>
       </c>
       <c r="B21" s="1">
-        <v>2.5388425480973301E-5</v>
+        <v>2.53883179274723E-5</v>
       </c>
       <c r="C21" s="1">
-        <v>9.1393660448066405E-5</v>
+        <v>9.1393273275251993E-5</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -655,10 +655,10 @@
         <v>15.3939393939394</v>
       </c>
       <c r="B22" s="1">
-        <v>2.5388425480973301E-5</v>
+        <v>2.53883179274723E-5</v>
       </c>
       <c r="C22" s="1">
-        <v>9.1393660448066405E-5</v>
+        <v>9.1393273275251993E-5</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -666,10 +666,10 @@
         <v>16.1636363636364</v>
       </c>
       <c r="B23" s="1">
-        <v>2.5388425480973399E-5</v>
+        <v>2.53883179274723E-5</v>
       </c>
       <c r="C23" s="1">
-        <v>9.1393660448066405E-5</v>
+        <v>9.1393273275251993E-5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -677,10 +677,10 @@
         <v>16.933333333333302</v>
       </c>
       <c r="B24" s="1">
-        <v>2.5388425480973399E-5</v>
+        <v>2.53883179274723E-5</v>
       </c>
       <c r="C24" s="1">
-        <v>9.1393660448066405E-5</v>
+        <v>9.1393273275251993E-5</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -688,10 +688,10 @@
         <v>17.7030303030303</v>
       </c>
       <c r="B25" s="1">
-        <v>2.5388425480973399E-5</v>
+        <v>2.53883179274723E-5</v>
       </c>
       <c r="C25" s="1">
-        <v>9.1393660448066405E-5</v>
+        <v>9.1393273275251993E-5</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -699,10 +699,10 @@
         <v>18.472727272727301</v>
       </c>
       <c r="B26" s="1">
-        <v>2.5388425480973399E-5</v>
+        <v>2.53883179274723E-5</v>
       </c>
       <c r="C26" s="1">
-        <v>9.1393660448066297E-5</v>
+        <v>9.1393273275251993E-5</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -710,10 +710,10 @@
         <v>19.2424242424242</v>
       </c>
       <c r="B27" s="1">
-        <v>2.5388425480973399E-5</v>
+        <v>2.53883179274723E-5</v>
       </c>
       <c r="C27" s="1">
-        <v>9.1393660448066297E-5</v>
+        <v>9.1393273275251993E-5</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -721,10 +721,10 @@
         <v>20.012121212121201</v>
       </c>
       <c r="B28" s="1">
-        <v>2.5388425480973399E-5</v>
+        <v>2.53883179274723E-5</v>
       </c>
       <c r="C28" s="1">
-        <v>9.1393660448066297E-5</v>
+        <v>9.1393273275251993E-5</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -732,10 +732,10 @@
         <v>20.781818181818199</v>
       </c>
       <c r="B29" s="1">
-        <v>2.5388425480973399E-5</v>
+        <v>2.53883179274723E-5</v>
       </c>
       <c r="C29" s="1">
-        <v>9.1393660448066297E-5</v>
+        <v>9.1393273275251993E-5</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -743,10 +743,10 @@
         <v>21.551515151515201</v>
       </c>
       <c r="B30" s="1">
-        <v>2.5388425480973399E-5</v>
+        <v>2.53883179274723E-5</v>
       </c>
       <c r="C30" s="1">
-        <v>9.1393660448066297E-5</v>
+        <v>9.1393273275251898E-5</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -754,10 +754,10 @@
         <v>22.321212121212099</v>
       </c>
       <c r="B31" s="1">
-        <v>2.5388425480973399E-5</v>
+        <v>2.53883179274723E-5</v>
       </c>
       <c r="C31" s="1">
-        <v>9.1393660448066202E-5</v>
+        <v>9.1393273275251898E-5</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -765,10 +765,10 @@
         <v>23.090909090909101</v>
       </c>
       <c r="B32" s="1">
-        <v>2.5388425480973399E-5</v>
+        <v>2.53883179274723E-5</v>
       </c>
       <c r="C32" s="1">
-        <v>9.1393660448066202E-5</v>
+        <v>9.1393273275251898E-5</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -776,10 +776,10 @@
         <v>23.860606060606099</v>
       </c>
       <c r="B33" s="1">
-        <v>2.5388425480973399E-5</v>
+        <v>2.53883179274723E-5</v>
       </c>
       <c r="C33" s="1">
-        <v>9.1393660448066202E-5</v>
+        <v>9.1393273275251898E-5</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -787,10 +787,10 @@
         <v>24.630303030303001</v>
       </c>
       <c r="B34" s="1">
-        <v>2.5388425480973399E-5</v>
+        <v>2.53883179274723E-5</v>
       </c>
       <c r="C34" s="1">
-        <v>9.1393660448066202E-5</v>
+        <v>9.1393273275251898E-5</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -798,10 +798,10 @@
         <v>25.4</v>
       </c>
       <c r="B35" s="1">
-        <v>2.5388425480973501E-5</v>
+        <v>2.53883179274723E-5</v>
       </c>
       <c r="C35" s="1">
-        <v>9.1393660448066202E-5</v>
+        <v>9.1393273275251898E-5</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -809,10 +809,10 @@
         <v>26.169696969697</v>
       </c>
       <c r="B36" s="1">
-        <v>2.5388425480973501E-5</v>
+        <v>2.53883179274723E-5</v>
       </c>
       <c r="C36" s="1">
-        <v>9.1393660448066202E-5</v>
+        <v>9.1393273275251898E-5</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -820,10 +820,10 @@
         <v>26.939393939393899</v>
       </c>
       <c r="B37" s="1">
-        <v>2.5388425480973501E-5</v>
+        <v>2.53883179274723E-5</v>
       </c>
       <c r="C37" s="1">
-        <v>9.1393660448066093E-5</v>
+        <v>9.1393273275251898E-5</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -831,10 +831,10 @@
         <v>27.7090909090909</v>
       </c>
       <c r="B38" s="1">
-        <v>2.5388425480973599E-5</v>
+        <v>2.53883179274723E-5</v>
       </c>
       <c r="C38" s="1">
-        <v>9.1393660448065998E-5</v>
+        <v>9.1393273275251993E-5</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -842,10 +842,10 @@
         <v>28.478787878787902</v>
       </c>
       <c r="B39" s="1">
-        <v>2.5388425480970801E-5</v>
+        <v>2.53883179274725E-5</v>
       </c>
       <c r="C39" s="1">
-        <v>9.1393660448068804E-5</v>
+        <v>9.1393273275251695E-5</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -853,10 +853,10 @@
         <v>29.2484848484848</v>
       </c>
       <c r="B40" s="1">
-        <v>2.5388425480909299E-5</v>
+        <v>2.53883179274842E-5</v>
       </c>
       <c r="C40" s="1">
-        <v>9.1393660448130305E-5</v>
+        <v>9.1393273275240094E-5</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -864,10 +864,10 @@
         <v>30.018181818181802</v>
       </c>
       <c r="B41" s="1">
-        <v>2.53884254803591E-5</v>
+        <v>2.5388317927607301E-5</v>
       </c>
       <c r="C41" s="1">
-        <v>9.1393660448680497E-5</v>
+        <v>9.1393273275116902E-5</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -875,10 +875,10 @@
         <v>30.7878787878788</v>
       </c>
       <c r="B42" s="1">
-        <v>2.5388425477566301E-5</v>
+        <v>2.5388317928286401E-5</v>
       </c>
       <c r="C42" s="1">
-        <v>9.1393660451473293E-5</v>
+        <v>9.1393273274437798E-5</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -886,10 +886,10 @@
         <v>31.557575757575801</v>
       </c>
       <c r="B43" s="1">
-        <v>2.5388425469367001E-5</v>
+        <v>2.5388317930351399E-5</v>
       </c>
       <c r="C43" s="1">
-        <v>9.13936604596726E-5</v>
+        <v>9.13932732723728E-5</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -897,10 +897,10 @@
         <v>32.3272727272727</v>
       </c>
       <c r="B44" s="1">
-        <v>2.5388425461614902E-5</v>
+        <v>2.5388317932049101E-5</v>
       </c>
       <c r="C44" s="1">
-        <v>9.1393660467424699E-5</v>
+        <v>9.1393273270675102E-5</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -908,10 +908,10 @@
         <v>33.096969696969701</v>
       </c>
       <c r="B45" s="1">
-        <v>2.53884255123187E-5</v>
+        <v>2.5388317916644401E-5</v>
       </c>
       <c r="C45" s="1">
-        <v>9.13936604167209E-5</v>
+        <v>9.1393273286079798E-5</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -919,10 +919,10 @@
         <v>33.866666666666703</v>
       </c>
       <c r="B46" s="1">
-        <v>2.5388425817925101E-5</v>
+        <v>2.53883178297155E-5</v>
       </c>
       <c r="C46" s="1">
-        <v>9.1393660111114395E-5</v>
+        <v>9.1393273373008703E-5</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -930,10 +930,10 @@
         <v>34.636363636363598</v>
       </c>
       <c r="B47" s="1">
-        <v>2.5388426764025101E-5</v>
+        <v>2.5388317579434099E-5</v>
       </c>
       <c r="C47" s="1">
-        <v>9.1393659165014398E-5</v>
+        <v>9.1393273623290106E-5</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -941,10 +941,10 @@
         <v>35.406060606060599</v>
       </c>
       <c r="B48" s="1">
-        <v>2.53884287055549E-5</v>
+        <v>2.5388317148762999E-5</v>
       </c>
       <c r="C48" s="1">
-        <v>9.1393657223484603E-5</v>
+        <v>9.1393274053961203E-5</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -952,10 +952,10 @@
         <v>36.175757575757601</v>
       </c>
       <c r="B49" s="1">
-        <v>2.53884312273053E-5</v>
+        <v>2.5388316893725099E-5</v>
       </c>
       <c r="C49" s="1">
-        <v>9.1393654701734203E-5</v>
+        <v>9.1393274308999205E-5</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -963,10 +963,10 @@
         <v>36.945454545454602</v>
       </c>
       <c r="B50" s="1">
-        <v>2.53884321003045E-5</v>
+        <v>2.5388317872652999E-5</v>
       </c>
       <c r="C50" s="1">
-        <v>9.1393653828735006E-5</v>
+        <v>9.1393273330071207E-5</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -974,10 +974,10 @@
         <v>37.715151515151497</v>
       </c>
       <c r="B51" s="1">
-        <v>2.5388427064962998E-5</v>
+        <v>2.5388321645493498E-5</v>
       </c>
       <c r="C51" s="1">
-        <v>9.1393658864076494E-5</v>
+        <v>9.13932695572307E-5</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
@@ -985,10 +985,10 @@
         <v>38.484848484848499</v>
       </c>
       <c r="B52" s="1">
-        <v>2.53884120210405E-5</v>
+        <v>2.53883288744859E-5</v>
       </c>
       <c r="C52" s="1">
-        <v>9.1393673907998996E-5</v>
+        <v>9.1393262328238298E-5</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
@@ -996,10 +996,10 @@
         <v>39.2545454545455</v>
       </c>
       <c r="B53" s="1">
-        <v>2.5388387835255202E-5</v>
+        <v>2.5388336916067499E-5</v>
       </c>
       <c r="C53" s="1">
-        <v>9.1393698093784301E-5</v>
+        <v>9.1393254286656805E-5</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
@@ -1007,10 +1007,10 @@
         <v>40.024242424242402</v>
       </c>
       <c r="B54" s="1">
-        <v>2.5388364758214299E-5</v>
+        <v>2.5388338333549899E-5</v>
       </c>
       <c r="C54" s="1">
-        <v>9.1393721170825203E-5</v>
+        <v>9.13932528691743E-5</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
@@ -1018,10 +1018,10 @@
         <v>40.793939393939397</v>
       </c>
       <c r="B55" s="1">
-        <v>2.53883610447568E-5</v>
+        <v>2.5388323294312201E-5</v>
       </c>
       <c r="C55" s="1">
-        <v>9.1393724884282696E-5</v>
+        <v>9.1393267908412005E-5</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -1029,10 +1029,10 @@
         <v>41.563636363636398</v>
       </c>
       <c r="B56" s="1">
-        <v>2.5388392620019698E-5</v>
+        <v>2.5388286990912299E-5</v>
       </c>
       <c r="C56" s="1">
-        <v>9.1393693309019798E-5</v>
+        <v>9.1393304211811894E-5</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
@@ -1040,10 +1040,10 @@
         <v>42.3333333333333</v>
       </c>
       <c r="B57" s="1">
-        <v>2.5388458120697398E-5</v>
+        <v>2.5388238439943E-5</v>
       </c>
       <c r="C57" s="1">
-        <v>9.1393627808341999E-5</v>
+        <v>9.1393352762781196E-5</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
@@ -1051,10 +1051,10 @@
         <v>43.103030303030302</v>
       </c>
       <c r="B58" s="1">
-        <v>2.5388530906498798E-5</v>
+        <v>2.53882028798465E-5</v>
       </c>
       <c r="C58" s="1">
-        <v>9.1393555022540606E-5</v>
+        <v>9.1393388322877703E-5</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
@@ -1062,10 +1062,10 @@
         <v>43.872727272727303</v>
       </c>
       <c r="B59" s="1">
-        <v>2.5388568585927999E-5</v>
+        <v>2.5388211608893699E-5</v>
       </c>
       <c r="C59" s="1">
-        <v>9.1393517343111395E-5</v>
+        <v>9.13933795938305E-5</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
@@ -1073,10 +1073,10 @@
         <v>44.642424242424298</v>
       </c>
       <c r="B60" s="1">
-        <v>2.5388538723808102E-5</v>
+        <v>2.5388281760474901E-5</v>
       </c>
       <c r="C60" s="1">
-        <v>9.1393547205231306E-5</v>
+        <v>9.1393309442249396E-5</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -1084,10 +1084,10 @@
         <v>45.4121212121212</v>
       </c>
       <c r="B61" s="1">
-        <v>2.53884446554823E-5</v>
+        <v>2.5388398522077299E-5</v>
       </c>
       <c r="C61" s="1">
-        <v>9.1393641273557094E-5</v>
+        <v>9.1393192680646893E-5</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -1095,10 +1095,10 @@
         <v>46.181818181818201</v>
       </c>
       <c r="B62" s="1">
-        <v>2.5388330946756898E-5</v>
+        <v>2.5388514553343102E-5</v>
       </c>
       <c r="C62" s="1">
-        <v>9.1393754982282499E-5</v>
+        <v>9.1393076649381094E-5</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
@@ -1106,10 +1106,10 @@
         <v>46.951515151515203</v>
       </c>
       <c r="B63" s="1">
-        <v>2.5388260383984398E-5</v>
+        <v>2.5388571575545501E-5</v>
       </c>
       <c r="C63" s="1">
-        <v>9.1393825545054799E-5</v>
+        <v>9.1393019627178704E-5</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
@@ -1117,10 +1117,10 @@
         <v>47.721212121212098</v>
       </c>
       <c r="B64" s="1">
-        <v>2.5388275496977399E-5</v>
+        <v>2.5388533142828799E-5</v>
       </c>
       <c r="C64" s="1">
-        <v>9.1393810432061897E-5</v>
+        <v>9.1393058059895403E-5</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -1128,10 +1128,10 @@
         <v>48.490909090909099</v>
       </c>
       <c r="B65" s="1">
-        <v>2.53883706920326E-5</v>
+        <v>2.53884077825619E-5</v>
       </c>
       <c r="C65" s="1">
-        <v>9.1393715237006703E-5</v>
+        <v>9.1393183420162302E-5</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -1139,10 +1139,10 @@
         <v>49.260606060606101</v>
       </c>
       <c r="B66" s="1">
-        <v>2.5388494766440699E-5</v>
+        <v>2.5388246591391402E-5</v>
       </c>
       <c r="C66" s="1">
-        <v>9.1393591162598498E-5</v>
+        <v>9.1393344611332794E-5</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
@@ -1150,10 +1150,10 @@
         <v>50.030303030303003</v>
       </c>
       <c r="B67" s="1">
-        <v>2.5388582172174399E-5</v>
+        <v>2.5388116144586399E-5</v>
       </c>
       <c r="C67" s="1">
-        <v>9.1393503756864901E-5</v>
+        <v>9.1393475058137899E-5</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
@@ -1161,10 +1161,10 @@
         <v>50.8</v>
       </c>
       <c r="B68" s="1">
-        <v>2.5388591412120101E-5</v>
+        <v>2.53880638595079E-5</v>
       </c>
       <c r="C68" s="1">
-        <v>9.13934945169193E-5</v>
+        <v>9.1393527343216306E-5</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
@@ -1172,10 +1172,10 @@
         <v>51.569696969696999</v>
       </c>
       <c r="B69" s="1">
-        <v>2.5388525402879601E-5</v>
+        <v>2.5388096872963002E-5</v>
       </c>
       <c r="C69" s="1">
-        <v>9.13935605261598E-5</v>
+        <v>9.1393494329761299E-5</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
@@ -1183,10 +1183,10 @@
         <v>52.339393939393901</v>
       </c>
       <c r="B70" s="1">
-        <v>2.5388423113867502E-5</v>
+        <v>2.5388185026043899E-5</v>
       </c>
       <c r="C70" s="1">
-        <v>9.1393662815171994E-5</v>
+        <v>9.13934061766803E-5</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
@@ -1194,10 +1194,10 @@
         <v>53.109090909090902</v>
       </c>
       <c r="B71" s="1">
-        <v>2.5388332129386702E-5</v>
+        <v>2.53882824507711E-5</v>
       </c>
       <c r="C71" s="1">
-        <v>9.13937537996527E-5</v>
+        <v>9.1393308751953106E-5</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
@@ -1205,10 +1205,10 @@
         <v>53.878787878787897</v>
       </c>
       <c r="B72" s="1">
-        <v>2.5388282654336099E-5</v>
+        <v>2.53883523032578E-5</v>
       </c>
       <c r="C72" s="1">
-        <v>9.1393803274703302E-5</v>
+        <v>9.1393238899466396E-5</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
@@ -1216,10 +1216,10 @@
         <v>54.648484848484898</v>
       </c>
       <c r="B73" s="1">
-        <v>2.53882784577226E-5</v>
+        <v>2.53883809155208E-5</v>
       </c>
       <c r="C73" s="1">
-        <v>9.1393807471316601E-5</v>
+        <v>9.1393210287203297E-5</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
@@ -1227,10 +1227,10 @@
         <v>55.4181818181818</v>
       </c>
       <c r="B74" s="1">
-        <v>2.53883055835484E-5</v>
+        <v>2.5388377246168601E-5</v>
       </c>
       <c r="C74" s="1">
-        <v>9.1393780345490601E-5</v>
+        <v>9.1393213956555297E-5</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
@@ -1238,10 +1238,10 @@
         <v>56.187878787878802</v>
       </c>
       <c r="B75" s="1">
-        <v>2.5388347762990502E-5</v>
+        <v>2.5388362664431199E-5</v>
       </c>
       <c r="C75" s="1">
-        <v>9.1393738166048303E-5</v>
+        <v>9.1393228538292698E-5</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
@@ -1249,10 +1249,10 @@
         <v>56.957575757575803</v>
       </c>
       <c r="B76" s="1">
-        <v>2.5388396437051201E-5</v>
+        <v>2.53883592808263E-5</v>
       </c>
       <c r="C76" s="1">
-        <v>9.1393689491987495E-5</v>
+        <v>9.1393231921897401E-5</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
@@ -1260,10 +1260,10 @@
         <v>57.727272727272698</v>
       </c>
       <c r="B77" s="1">
-        <v>2.5388451566647801E-5</v>
+        <v>2.53883828251801E-5</v>
       </c>
       <c r="C77" s="1">
-        <v>9.1393634362390698E-5</v>
+        <v>9.1393208377543503E-5</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
@@ -1271,10 +1271,10 @@
         <v>58.4969696969697</v>
       </c>
       <c r="B78" s="1">
-        <v>2.53885189840901E-5</v>
+        <v>2.5388442672653299E-5</v>
       </c>
       <c r="C78" s="1">
-        <v>9.1393566944948301E-5</v>
+        <v>9.1393148530070402E-5</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
@@ -1282,10 +1282,10 @@
         <v>59.266666666666701</v>
       </c>
       <c r="B79" s="1">
-        <v>2.5388614259683701E-5</v>
+        <v>2.5388550486567E-5</v>
       </c>
       <c r="C79" s="1">
-        <v>9.1393471669354694E-5</v>
+        <v>9.1393040716156694E-5</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
@@ -1293,10 +1293,10 @@
         <v>60.036363636363603</v>
       </c>
       <c r="B80" s="1">
-        <v>2.5388781831415199E-5</v>
+        <v>2.5388741141504401E-5</v>
       </c>
       <c r="C80" s="1">
-        <v>9.1393304097622799E-5</v>
+        <v>9.1392850061219598E-5</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
@@ -1304,10 +1304,10 @@
         <v>60.806060606060598</v>
       </c>
       <c r="B81" s="1">
-        <v>2.5389137813458101E-5</v>
+        <v>2.5389115669376201E-5</v>
       </c>
       <c r="C81" s="1">
-        <v>9.1392948115579396E-5</v>
+        <v>9.1392475533348195E-5</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
@@ -1315,10 +1315,10 @@
         <v>61.575757575757599</v>
       </c>
       <c r="B82" s="1">
-        <v>2.5389955135194701E-5</v>
+        <v>2.5389929218777001E-5</v>
       </c>
       <c r="C82" s="1">
-        <v>9.1392130793841898E-5</v>
+        <v>9.1391661983947998E-5</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
@@ -1326,10 +1326,10 @@
         <v>62.345454545454501</v>
       </c>
       <c r="B83" s="1">
-        <v>2.53918419236739E-5</v>
+        <v>2.5391776585924502E-5</v>
       </c>
       <c r="C83" s="1">
-        <v>9.1390244005361398E-5</v>
+        <v>9.13898146168011E-5</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
@@ -1337,10 +1337,10 @@
         <v>63.115151515151503</v>
       </c>
       <c r="B84" s="1">
-        <v>2.5396135264995601E-5</v>
+        <v>2.5395993179506901E-5</v>
       </c>
       <c r="C84" s="1">
-        <v>9.1385950664038396E-5</v>
+        <v>9.1385598023219195E-5</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
@@ -1348,10 +1348,10 @@
         <v>63.884848484848497</v>
       </c>
       <c r="B85" s="1">
-        <v>2.5405777552880499E-5</v>
+        <v>2.5405529863662601E-5</v>
       </c>
       <c r="C85" s="1">
-        <v>9.1376308376152495E-5</v>
+        <v>9.1376061339063305E-5</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
@@ -1359,10 +1359,10 @@
         <v>64.654545454545499</v>
       </c>
       <c r="B86" s="1">
-        <v>2.54272428159953E-5</v>
+        <v>2.5426860924105501E-5</v>
       </c>
       <c r="C86" s="1">
-        <v>9.1354843113037806E-5</v>
+        <v>9.1354730278620094E-5</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
@@ -1370,10 +1370,10 @@
         <v>65.424242424242394</v>
       </c>
       <c r="B87" s="1">
-        <v>2.5474722343293901E-5</v>
+        <v>2.54741346892662E-5</v>
       </c>
       <c r="C87" s="1">
-        <v>9.1307363585740899E-5</v>
+        <v>9.1307456513458802E-5</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
@@ -1381,10 +1381,10 @@
         <v>66.193939393939402</v>
       </c>
       <c r="B88" s="1">
-        <v>2.5579152712950199E-5</v>
+        <v>2.5578166579979301E-5</v>
       </c>
       <c r="C88" s="1">
-        <v>9.1202933216086803E-5</v>
+        <v>9.1203424622744099E-5</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
@@ -1392,10 +1392,10 @@
         <v>66.963636363636397</v>
       </c>
       <c r="B89" s="1">
-        <v>2.5807513180777799E-5</v>
+        <v>2.5805715471607999E-5</v>
       </c>
       <c r="C89" s="1">
-        <v>9.0974572748265102E-5</v>
+        <v>9.0975875731117101E-5</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
@@ -1403,10 +1403,10 @@
         <v>67.733333333333306</v>
       </c>
       <c r="B90" s="1">
-        <v>2.6303278766130001E-5</v>
+        <v>2.6299856230582699E-5</v>
       </c>
       <c r="C90" s="1">
-        <v>9.0478807162919399E-5</v>
+        <v>9.0481734972144902E-5</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
@@ -1414,10 +1414,10 @@
         <v>68.5030303030303</v>
       </c>
       <c r="B91" s="1">
-        <v>2.7366907305291999E-5</v>
+        <v>2.7360169442571501E-5</v>
       </c>
       <c r="C91" s="1">
-        <v>8.9415178623762696E-5</v>
+        <v>8.9421421760138E-5</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
@@ -1425,10 +1425,10 @@
         <v>69.272727272727295</v>
       </c>
       <c r="B92" s="1">
-        <v>2.9595512555573299E-5</v>
+        <v>2.95819781548241E-5</v>
       </c>
       <c r="C92" s="1">
-        <v>8.7186573373498896E-5</v>
+        <v>8.7199613047896494E-5</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
@@ -1436,10 +1436,10 @@
         <v>70.042424242424303</v>
       </c>
       <c r="B93" s="1">
-        <v>3.4044074633847897E-5</v>
+        <v>3.4017775663906602E-5</v>
       </c>
       <c r="C93" s="1">
-        <v>8.2738011295242797E-5</v>
+        <v>8.2763815538812406E-5</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
@@ -1447,10 +1447,10 @@
         <v>70.812121212121198</v>
       </c>
       <c r="B94" s="1">
-        <v>4.2140340176654301E-5</v>
+        <v>4.2094678261941397E-5</v>
       </c>
       <c r="C94" s="1">
-        <v>7.4641745752434705E-5</v>
+        <v>7.4686912940745106E-5</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
@@ -1458,10 +1458,10 @@
         <v>71.581818181818207</v>
       </c>
       <c r="B95" s="1">
-        <v>5.4766658491963197E-5</v>
+        <v>5.4701249705433797E-5</v>
       </c>
       <c r="C95" s="1">
-        <v>6.2015427437105304E-5</v>
+        <v>6.2080341497191299E-5</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
@@ -1469,10 +1469,10 @@
         <v>72.351515151515201</v>
       </c>
       <c r="B96" s="1">
-        <v>7.0631170966025701E-5</v>
+        <v>7.0557914585330303E-5</v>
       </c>
       <c r="C96" s="1">
-        <v>4.6150914963060798E-5</v>
+        <v>4.6223676617266197E-5</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
@@ -1480,10 +1480,10 @@
         <v>73.121212121212096</v>
       </c>
       <c r="B97" s="1">
-        <v>8.6220564533467605E-5</v>
+        <v>8.6156513803473204E-5</v>
       </c>
       <c r="C97" s="1">
-        <v>3.0561521395737201E-5</v>
+        <v>3.06250773992076E-5</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
@@ -1491,10 +1491,10 @@
         <v>73.890909090909105</v>
       </c>
       <c r="B98" s="1">
-        <v>9.8430967686638697E-5</v>
+        <v>9.8385038835969706E-5</v>
       </c>
       <c r="C98" s="1">
-        <v>1.8351118242649498E-5</v>
+        <v>1.8396552366855998E-5</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
@@ -1502,10 +1502,10 @@
         <v>74.660606060606099</v>
       </c>
       <c r="B99">
-        <v>1.06472604137322E-4</v>
+        <v>1.06443643350913E-4</v>
       </c>
       <c r="C99" s="1">
-        <v>1.03094817919387E-5</v>
+        <v>1.03379478520468E-5</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
@@ -1513,10 +1513,10 @@
         <v>75.430303030302994</v>
       </c>
       <c r="B100">
-        <v>1.11198727782416E-4</v>
+        <v>1.11181643703792E-4</v>
       </c>
       <c r="C100" s="1">
-        <v>5.5833581468052998E-6</v>
+        <v>5.5999474992807397E-6</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
@@ -1524,10 +1524,10 @@
         <v>76.2</v>
       </c>
       <c r="B101">
-        <v>1.1379600485436E-4</v>
+        <v>1.13786138314579E-4</v>
       </c>
       <c r="C101" s="1">
-        <v>2.9860810747497701E-6</v>
+        <v>2.9954528885300598E-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>